<commit_message>
Added several new requirements written in English. For our next phase we should have this document ready and fully in English.
Signed-off-by: raviv <ravivkomem@gmail.com>
</commit_message>
<xml_diff>
--- a/מסמך דרישות- עידו.xlsx
+++ b/מסמך דרישות- עידו.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5802D5AB-CA54-4CAA-90BD-2F880CEA5E71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18270" windowHeight="13635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="56">
   <si>
     <t>זיהוי דרישה</t>
   </si>
@@ -175,12 +176,24 @@
   </si>
   <si>
     <t xml:space="preserve">המערכת תאפשר הפקת אישור שהתהליך הסתיים בהצלחה </t>
+  </si>
+  <si>
+    <t>The system shall have different user premissions</t>
+  </si>
+  <si>
+    <t>System premissions shall be: Student, Lecturer, Worker, Department Head, Admin</t>
+  </si>
+  <si>
+    <t>Log in action requires two fields: user name, password</t>
+  </si>
+  <si>
+    <t>Each user shall have unique user name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -215,7 +228,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,6 +248,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -283,7 +302,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
@@ -304,6 +323,10 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="3" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,21 +609,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.8984375" customWidth="1"/>
-    <col min="2" max="2" width="87.8984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.8984375" customWidth="1"/>
+    <col min="1" max="1" width="12.875" customWidth="1"/>
+    <col min="2" max="2" width="87.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -611,7 +634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -622,7 +645,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>1.1000000000000001</v>
       </c>
@@ -633,565 +656,591 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="11"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
         <v>1.2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="C6" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
         <v>1.3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="C7" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
         <v>2</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="C8" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
         <v>2.1</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="C9" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="C11" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
         <v>2.4</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="C12" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="7">
         <v>2.5</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>3</v>
-      </c>
-      <c r="B12" s="4" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>3</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+      <c r="C14" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
         <v>3.1</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B15" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="C15" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
         <v>4</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+      <c r="C16" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="C17" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
         <v>5</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+      <c r="C18" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="9">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B19" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
-        <v>6</v>
-      </c>
-      <c r="B18" s="4" t="s">
+      <c r="C19" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>6</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
+      <c r="C20" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="7">
         <v>6.1</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B21" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+      <c r="C21" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
         <v>7</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
+      <c r="C22" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="7">
         <v>7.1</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B23" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
+      <c r="C23" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
         <v>8</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
+      <c r="C24" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
         <v>9</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+      <c r="C25" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
         <v>10</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
+      <c r="C26" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="9">
         <v>10.1</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B27" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
+      <c r="C27" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
         <v>10.199999999999999</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
+      <c r="C28" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="9">
         <v>10.3</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B29" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
+      <c r="C29" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
         <v>11</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
+      <c r="C30" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
         <v>12</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B31" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
+      <c r="C31" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
         <v>13</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="9">
+      <c r="C32" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="9">
         <v>13.1</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B33" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="9">
+      <c r="C33" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="9">
         <v>13.2</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B34" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
+      <c r="C34" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
         <v>14</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
+      <c r="C35" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="3">
         <v>15</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B36" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="9">
+      <c r="C36" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="9">
         <v>15.1</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B37" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="9">
+      <c r="C37" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="9">
         <v>15.2</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B38" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
+      <c r="C38" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="3">
         <v>16</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B39" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
+      <c r="C39" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="3">
         <v>16.100000000000001</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B40" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="9">
+      <c r="C40" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="9">
         <v>16.2</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B41" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="3">
+      <c r="C41" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="3">
         <v>17</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B42" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="9">
+      <c r="C42" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="9">
         <v>17.100000000000001</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B43" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="3">
+      <c r="C43" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="3">
         <v>17.2</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B44" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="3">
+      <c r="C44" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="3">
         <v>17.3</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B45" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="3">
+      <c r="C45" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="3">
         <v>17.399999999999999</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B46" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="3">
+      <c r="C46" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="3">
         <v>17.5</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B47" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="9">
+      <c r="C47" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="9">
         <v>17.600000000000001</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B48" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C46" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="3">
+      <c r="C48" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="3">
         <v>18</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B49" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C49" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>19</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>